<commit_message>
Avance administración de noticias y anuncios
</commit_message>
<xml_diff>
--- a/docs/matriz_de_requisitos.xlsx
+++ b/docs/matriz_de_requisitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\SHAIR\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBE24CD-5FCF-458F-B8A1-B86D47965E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F467E4E8-C7B3-4889-BF1A-924A569DAD81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -433,7 +433,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -515,6 +515,11 @@
       <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="14">
@@ -827,17 +832,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -852,14 +855,11 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -870,69 +870,18 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -942,62 +891,117 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="13" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1044,6 +1048,938 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="50"/>
+      <c:rotY val="0"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="0"/>
+      <c:perspective val="60"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="threePt" dir="t"/>
+              </a:scene3d>
+              <a:sp3d prstMaterial="matte"/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="threePt" dir="t"/>
+              </a:scene3d>
+              <a:sp3d prstMaterial="matte"/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-E423-4D47-A50D-E9AEC4B4FEF1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-CO"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>' RF'!$A$36:$A$37</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Total de requisitos</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Total completados</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>' RF'!$B$36:$B$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E423-4D47-A50D-E9AEC4B4FEF1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="78000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:pattFill prst="dkDnDiag">
+      <a:fgClr>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:fgClr>
+      <a:bgClr>
+        <a:schemeClr val="lt1"/>
+      </a:bgClr>
+    </a:pattFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="261">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="dkDnDiag">
+        <a:fgClr>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="lt1"/>
+        </a:bgClr>
+      </a:pattFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="317500" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="25000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="88900" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="threePt" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="matte"/>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:alpha val="78000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1562100</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>6134100</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F2CFCD7-857D-7E7A-67FB-AA1E505E9402}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1345,530 +2281,530 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="126.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="27" width="9.42578125" style="3" customWidth="1"/>
-    <col min="28" max="16384" width="15.140625" style="3"/>
+    <col min="1" max="1" width="23.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="126.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="27" width="9.42578125" style="2" customWidth="1"/>
+    <col min="28" max="16384" width="15.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="27"/>
+      <c r="B4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="27"/>
+      <c r="B5" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="27"/>
+      <c r="B6" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="10" t="s">
+      <c r="A7" s="27"/>
+      <c r="B7" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="27"/>
+      <c r="B8" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="14"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="11"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="27"/>
+      <c r="B9" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
+      <c r="F9" s="6"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6" t="s">
+      <c r="A10" s="27"/>
+      <c r="B10" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
-      <c r="B13" s="6" t="s">
+      <c r="A13" s="25"/>
+      <c r="B13" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="25"/>
+      <c r="B14" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="6" t="s">
+      <c r="A15" s="25"/>
+      <c r="B15" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="F15" s="7"/>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="10" t="s">
+      <c r="A16" s="25"/>
+      <c r="B16" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="F16" s="7"/>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
-      <c r="B17" s="10" t="s">
+      <c r="A17" s="25"/>
+      <c r="B17" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="F17" s="7"/>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
-      <c r="B18" s="10" t="s">
+      <c r="A18" s="25"/>
+      <c r="B18" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="F18" s="7"/>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="6" t="s">
+      <c r="A19" s="26"/>
+      <c r="B19" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="F19" s="7"/>
+      <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="23"/>
-      <c r="F20" s="7"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="30"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="F21" s="7"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="10" t="s">
+      <c r="A22" s="27"/>
+      <c r="B22" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="F22" s="7"/>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="10" t="s">
+      <c r="A23" s="27"/>
+      <c r="B23" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="F23" s="7"/>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="10" t="s">
+      <c r="A24" s="27"/>
+      <c r="B24" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="F24" s="7"/>
+      <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6" t="s">
+      <c r="A25" s="27"/>
+      <c r="B25" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="10" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="23"/>
+      <c r="A26" s="28"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="30"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="10" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
-      <c r="B28" s="10" t="s">
+      <c r="A28" s="33"/>
+      <c r="B28" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="10" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
-      <c r="B29" s="10" t="s">
+      <c r="A29" s="33"/>
+      <c r="B29" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="8" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
-      <c r="B30" s="10" t="s">
+      <c r="A30" s="33"/>
+      <c r="B30" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="8" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="26"/>
-      <c r="B31" s="6" t="s">
+      <c r="A31" s="34"/>
+      <c r="B31" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="10" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="23"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="30"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="5" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="28"/>
-      <c r="B34" s="10" t="s">
+      <c r="A34" s="36"/>
+      <c r="B34" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="8" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
-      <c r="B35" s="22"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="23"/>
+      <c r="A35" s="28"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="30"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="29" t="s">
+      <c r="A36" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="B36" s="30">
+      <c r="B36" s="4">
         <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="B37" s="30">
-        <v>16</v>
+      <c r="B37" s="4">
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="B38" s="30">
-        <f>(B37*B36)/B36</f>
-        <v>16</v>
+      <c r="B38" s="52">
+        <f>B37/B36</f>
+        <v>0.6428571428571429</v>
       </c>
     </row>
   </sheetData>
@@ -1878,16 +2814,17 @@
     <mergeCell ref="A27:A31"/>
     <mergeCell ref="A35:D35"/>
     <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A1:D1"/>
     <mergeCell ref="A12:A19"/>
     <mergeCell ref="A21:A25"/>
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="A3:A10"/>
     <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1901,66 +2838,66 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10" style="34" customWidth="1"/>
-    <col min="5" max="5" width="82.28515625" style="34" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" style="34" bestFit="1" customWidth="1"/>
-    <col min="7" max="26" width="9.42578125" style="34" customWidth="1"/>
-    <col min="27" max="16384" width="15.140625" style="34"/>
+    <col min="1" max="1" width="9" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10" style="15" customWidth="1"/>
+    <col min="5" max="5" width="82.28515625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="26" width="9.42578125" style="15" customWidth="1"/>
+    <col min="27" max="16384" width="15.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="33"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="44"/>
     </row>
     <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="42" t="s">
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="19" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="43" t="s">
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="37" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="43"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="37"/>
     </row>
     <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="21" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="49" t="s">
@@ -1969,12 +2906,12 @@
       <c r="C5" s="49"/>
       <c r="D5" s="49"/>
       <c r="E5" s="49"/>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="48" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="21" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="49" t="s">
@@ -1983,24 +2920,24 @@
       <c r="C6" s="49"/>
       <c r="D6" s="49"/>
       <c r="E6" s="49"/>
-      <c r="F6" s="35"/>
+      <c r="F6" s="48"/>
     </row>
     <row r="7" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="43" t="s">
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="37" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="21" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="49" t="s">
@@ -2009,10 +2946,10 @@
       <c r="C8" s="49"/>
       <c r="D8" s="49"/>
       <c r="E8" s="49"/>
-      <c r="F8" s="43"/>
+      <c r="F8" s="37"/>
     </row>
     <row r="9" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="49" t="s">
@@ -2021,12 +2958,12 @@
       <c r="C9" s="49"/>
       <c r="D9" s="49"/>
       <c r="E9" s="49"/>
-      <c r="F9" s="36" t="s">
+      <c r="F9" s="17" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="22" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="51" t="s">
@@ -2035,91 +2972,91 @@
       <c r="C10" s="51"/>
       <c r="D10" s="51"/>
       <c r="E10" s="51"/>
-      <c r="F10" s="43" t="s">
+      <c r="F10" s="37" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="52" t="s">
+      <c r="B11" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="43"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="37"/>
     </row>
     <row r="12" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="37" t="s">
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="16" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="43" t="s">
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="37" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="50" t="s">
+      <c r="A14" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="53" t="s">
+      <c r="B14" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="43"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="37"/>
     </row>
     <row r="15" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="35" t="s">
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="48" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="44" t="s">
+      <c r="A16" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="35"/>
-    </row>
-    <row r="17" s="34" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="34" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="34" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="48"/>
+    </row>
+    <row r="17" s="15" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="15" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="15" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
     <mergeCell ref="A1:F1"/>

</xml_diff>